<commit_message>
RTE Pdf export sample
</commit_message>
<xml_diff>
--- a/Promised Incidents.xlsx
+++ b/Promised Incidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SyncfusionSupport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E500C653-5425-4C56-AD8B-9FA0748092C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBE3D7F-CA35-48CB-A283-A8B2E204153A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DA94DFC5-6F67-4698-9BB4-4B99735D4326}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>Control</t>
   </si>
@@ -42,9 +39,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Feedback- 11311</t>
-  </si>
-  <si>
     <t>EjsTreeView - NodeTemplate is Not Handling Context Item Enums Correctly </t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>EJ1</t>
   </si>
   <si>
-    <t>contextMenu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Feb 2 week </t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>EJ1/EJ2</t>
   </si>
   <si>
-    <t>Promised Date/Patch</t>
-  </si>
-  <si>
     <t>Freeze Filter selection</t>
   </si>
   <si>
@@ -123,9 +111,6 @@
     <t>Unable to start ASP.Net MVC webapp after adding nuget package syncfusion.aspnet.mvc5</t>
   </si>
   <si>
-    <t>listbox</t>
-  </si>
-  <si>
     <t>ejListBox reset data source and enableIncrementalSearch</t>
   </si>
   <si>
@@ -156,7 +141,28 @@
     <t>List box doesn't show 'false' string</t>
   </si>
   <si>
-    <t>Muthu</t>
+    <t>Updated Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>F11311</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ContextMenu</t>
+  </si>
+  <si>
+    <t>Promised Date /Patch</t>
   </si>
 </sst>
 </file>
@@ -256,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -313,9 +319,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -325,13 +328,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,364 +656,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD306F89-E025-408D-9D47-2862068C9AD7}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.90625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6328125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="9"/>
-    <col min="7" max="7" width="13.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="9"/>
+    <col min="5" max="5" width="13.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>261028</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="7">
+        <v>43873</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>263245</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="7">
         <v>43866</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="7">
+        <v>43867</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>262595</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7">
         <v>43881</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="7">
+        <v>43881</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>264330</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="7">
         <v>43886</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="7">
+        <v>43885</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>261830</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7">
         <v>43886</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="7">
+        <v>43886</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>266148</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7">
         <v>43889</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="7">
+        <v>43889</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>266699</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E9" s="14">
         <v>43887</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="14">
+        <v>43887</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>263939</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>267451</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="7">
+        <v>43903</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="7">
+        <v>43906</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>264330</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="7">
+        <v>43903</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="7">
+        <v>43906</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="25">
+        <v>152199</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>267451</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="27">
-        <v>43903</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>264330</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="27">
-        <v>43903</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="8">
-        <v>152199</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>152235</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="10">
         <v>43915</v>
       </c>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="21">
+      <c r="F14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="28">
         <v>267451</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="29">
+        <v>43908</v>
+      </c>
+      <c r="F15" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="23">
-        <v>43908</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21">
+      <c r="G15" s="29">
+        <v>43906</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20">
         <v>269285</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="23">
+      <c r="B16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="22">
         <v>43914</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>